<commit_message>
git add Evie Marginson- 469104- Premier League Data Analyser.ipynb
</commit_message>
<xml_diff>
--- a/Data/Luton Stats.xlsx
+++ b/Data/Luton Stats.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -629,6 +629,106 @@
         <v>71</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>23/24</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Luton</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>18</v>
+      </c>
+      <c r="D5" t="n">
+        <v>26</v>
+      </c>
+      <c r="E5" t="n">
+        <v>38</v>
+      </c>
+      <c r="F5" t="n">
+        <v>6</v>
+      </c>
+      <c r="G5" t="n">
+        <v>24</v>
+      </c>
+      <c r="H5" t="n">
+        <v>8</v>
+      </c>
+      <c r="I5" t="n">
+        <v>52</v>
+      </c>
+      <c r="J5" t="n">
+        <v>85</v>
+      </c>
+      <c r="K5" t="n">
+        <v>-33</v>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Carlton Morris</t>
+        </is>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>23/24</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Luton</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>18</v>
+      </c>
+      <c r="D6" t="n">
+        <v>26</v>
+      </c>
+      <c r="E6" t="n">
+        <v>38</v>
+      </c>
+      <c r="F6" t="n">
+        <v>6</v>
+      </c>
+      <c r="G6" t="n">
+        <v>24</v>
+      </c>
+      <c r="H6" t="n">
+        <v>8</v>
+      </c>
+      <c r="I6" t="n">
+        <v>52</v>
+      </c>
+      <c r="J6" t="n">
+        <v>85</v>
+      </c>
+      <c r="K6" t="n">
+        <v>-33</v>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Carlton Morris</t>
+        </is>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>71</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>